<commit_message>
Updated lesson 9, added some content to 8
</commit_message>
<xml_diff>
--- a/07. Python and Excel/costs_and_prices.xlsx
+++ b/07. Python and Excel/costs_and_prices.xlsx
@@ -46,6 +46,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="&quot;EUR &quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="&quot;GBP &quot;#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="&quot;CNY &quot;#,##0.00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,9 +85,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,12 +396,14 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -412,43 +422,56 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>30</v>
+      </c>
+      <c r="C2" s="4">
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>12</v>
+      </c>
+      <c r="C3" s="4">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>1.75</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>7.5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>